<commit_message>
chore: (normalization) added support for managers table in the frontend
</commit_message>
<xml_diff>
--- a/Test Files/data.xlsx
+++ b/Test Files/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Senior Developer</t>
   </si>
   <si>
-    <t>Michael</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Frontend Developer</t>
   </si>
   <si>
-    <t>David</t>
-  </si>
-  <si>
     <t>Project Alpha,Project Theta</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Jane Smith</t>
   </si>
   <si>
-    <t>Emily</t>
-  </si>
-  <si>
     <t>React,Angular</t>
   </si>
   <si>
@@ -129,10 +120,10 @@
     <t>Chris Evans</t>
   </si>
   <si>
-    <t>Sarah</t>
-  </si>
-  <si>
     <t>chris.evans@example.com</t>
+  </si>
+  <si>
+    <t>Rajesh</t>
   </si>
 </sst>
 </file>
@@ -454,7 +445,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,156 +490,156 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
       </c>
       <c r="I2" s="1">
         <v>44530</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
       </c>
       <c r="I3" s="1">
         <v>44938</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
       </c>
       <c r="I4" s="1">
         <v>44976</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1">
         <v>44898</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I6" s="1">
         <v>43938</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>